<commit_message>
updated sample array values
</commit_message>
<xml_diff>
--- a/Sample array values.xlsx
+++ b/Sample array values.xlsx
@@ -47,13 +47,13 @@
     <t>ellipse(x[0],y[0],diam[0],diam[0])</t>
   </si>
   <si>
-    <t>ellipse(500,400,50,50)</t>
-  </si>
-  <si>
     <t>ellipse(x[1],y[1],diam[1],diam[1])</t>
   </si>
   <si>
-    <t>ellipse(225,150,20,20)</t>
+    <t>ellipse(562,419,16,16)</t>
+  </si>
+  <si>
+    <t>ellipse(162,389,29,29)</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" t="s">
         <v>9</v>

</xml_diff>